<commit_message>
updated ATMEL chip pin allocation.
</commit_message>
<xml_diff>
--- a/parts/MCU_atmega328p/arduino_2_328_PinOut.xlsx
+++ b/parts/MCU_atmega328p/arduino_2_328_PinOut.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27760" yWindow="400" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="16580" yWindow="1000" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>arduino pin</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>ethernet pin 5</t>
+  </si>
+  <si>
+    <t>27-PC4</t>
+  </si>
+  <si>
+    <t>28-PC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solonoid </t>
+  </si>
+  <si>
+    <t>LCD-!RST</t>
   </si>
 </sst>
 </file>
@@ -540,7 +552,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -616,6 +628,9 @@
       <c r="B9" t="s">
         <v>9</v>
       </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3">
@@ -624,6 +639,9 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3">
@@ -716,8 +734,8 @@
       <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="3">
-        <v>27</v>
+      <c r="B21" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -727,8 +745,8 @@
       <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="3">
-        <v>28</v>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -780,7 +798,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>